<commit_message>
daily_stats method for compare
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -265,10 +265,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.14"/>
@@ -405,7 +405,7 @@
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.99"/>
   </cols>

</xml_diff>